<commit_message>
handle array object and refactor createFiles method
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28409"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{513DD5A9-5D36-423E-9D25-067DE9CACB84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{64BE398A-8F78-40DD-8F88-9C603F9E3485}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="56">
   <si>
     <t>key</t>
   </si>
@@ -67,6 +67,129 @@
     <t>nessuna mela | una mela | {count} mele</t>
   </si>
   <si>
+    <t>a.b.list[1].x</t>
+  </si>
+  <si>
+    <t>a b list 1 x</t>
+  </si>
+  <si>
+    <t>a b リスト 1 x</t>
+  </si>
+  <si>
+    <t>a b elenco 1 x</t>
+  </si>
+  <si>
+    <t>a.b.list[1].y</t>
+  </si>
+  <si>
+    <t>a b list 1 y</t>
+  </si>
+  <si>
+    <t>a b リスト 1 y</t>
+  </si>
+  <si>
+    <t>a b elenco 1 y</t>
+  </si>
+  <si>
+    <t>a.b.list[2]</t>
+  </si>
+  <si>
+    <t>a b list 2</t>
+  </si>
+  <si>
+    <t>a b リスト 2</t>
+  </si>
+  <si>
+    <t>a b elenco 2</t>
+  </si>
+  <si>
+    <t>a.d</t>
+  </si>
+  <si>
+    <t>this is a "test"</t>
+  </si>
+  <si>
+    <t>これは "テスト" です</t>
+  </si>
+  <si>
+    <t>questo è un "test"</t>
+  </si>
+  <si>
+    <t>x.1</t>
+  </si>
+  <si>
+    <t>car | cars</t>
+  </si>
+  <si>
+    <t>macchina | automobili</t>
+  </si>
+  <si>
+    <t>x.2</t>
+  </si>
+  <si>
+    <t>x 2</t>
+  </si>
+  <si>
+    <t>x.5</t>
+  </si>
+  <si>
+    <t>x 5\nnewline</t>
+  </si>
+  <si>
+    <t>x 5\n改行</t>
+  </si>
+  <si>
+    <t>y</t>
+  </si>
+  <si>
+    <t>test&lt;br&gt;y</t>
+  </si>
+  <si>
+    <t>テスト&lt;br&gt;y</t>
+  </si>
+  <si>
+    <t>z[0]</t>
+  </si>
+  <si>
+    <t>z0</t>
+  </si>
+  <si>
+    <t>z0 ja</t>
+  </si>
+  <si>
+    <t>z0 it</t>
+  </si>
+  <si>
+    <t>z[1]</t>
+  </si>
+  <si>
+    <t>z1</t>
+  </si>
+  <si>
+    <t>z1 ja</t>
+  </si>
+  <si>
+    <t>z1 it</t>
+  </si>
+  <si>
+    <t>z[2]</t>
+  </si>
+  <si>
+    <t>z2</t>
+  </si>
+  <si>
+    <t>z2 ja</t>
+  </si>
+  <si>
+    <t>z2 it</t>
+  </si>
+  <si>
+    <t>lang</t>
+  </si>
+  <si>
+    <t>a.b</t>
+  </si>
+  <si>
     <t>a.b.list[1]</t>
   </si>
   <si>
@@ -77,57 +200,6 @@
   </si>
   <si>
     <t>a b elenco 1</t>
-  </si>
-  <si>
-    <t>a.d</t>
-  </si>
-  <si>
-    <t>this is a "test"</t>
-  </si>
-  <si>
-    <t>これは "テスト" です</t>
-  </si>
-  <si>
-    <t>questo è un "test"</t>
-  </si>
-  <si>
-    <t>x.1</t>
-  </si>
-  <si>
-    <t>car | cars</t>
-  </si>
-  <si>
-    <t>macchina | automobili</t>
-  </si>
-  <si>
-    <t>x.2</t>
-  </si>
-  <si>
-    <t>x 2</t>
-  </si>
-  <si>
-    <t>x.5</t>
-  </si>
-  <si>
-    <t>x 5\nnewline</t>
-  </si>
-  <si>
-    <t>x 5\n改行</t>
-  </si>
-  <si>
-    <t>y</t>
-  </si>
-  <si>
-    <t>test&lt;br&gt;y</t>
-  </si>
-  <si>
-    <t>テスト&lt;br&gt;y</t>
-  </si>
-  <si>
-    <t>lang</t>
-  </si>
-  <si>
-    <t>a.b</t>
   </si>
 </sst>
 </file>
@@ -507,9 +579,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:D15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -617,52 +691,122 @@
         <v>20</v>
       </c>
       <c r="C7" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D7" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B8" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C8" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="D8" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="B9" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="C9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="D9" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="B10" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="C10" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="D10" t="s">
-        <v>28</v>
+        <v>31</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" t="s">
+        <v>32</v>
+      </c>
+      <c r="B11" t="s">
+        <v>33</v>
+      </c>
+      <c r="C11" t="s">
+        <v>34</v>
+      </c>
+      <c r="D11" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" t="s">
+        <v>35</v>
+      </c>
+      <c r="B12" t="s">
+        <v>36</v>
+      </c>
+      <c r="C12" t="s">
+        <v>37</v>
+      </c>
+      <c r="D12" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" t="s">
+        <v>38</v>
+      </c>
+      <c r="B13" t="s">
+        <v>39</v>
+      </c>
+      <c r="C13" t="s">
+        <v>40</v>
+      </c>
+      <c r="D13" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" t="s">
+        <v>42</v>
+      </c>
+      <c r="B14" t="s">
+        <v>43</v>
+      </c>
+      <c r="C14" t="s">
+        <v>44</v>
+      </c>
+      <c r="D14" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" t="s">
+        <v>46</v>
+      </c>
+      <c r="B15" t="s">
+        <v>47</v>
+      </c>
+      <c r="C15" t="s">
+        <v>48</v>
+      </c>
+      <c r="D15" t="s">
+        <v>49</v>
       </c>
     </row>
   </sheetData>
@@ -686,13 +830,13 @@
   <sheetData>
     <row r="1" spans="1:10">
       <c r="A1" t="s">
-        <v>30</v>
+        <v>50</v>
       </c>
       <c r="B1" t="s">
         <v>4</v>
       </c>
       <c r="C1" t="s">
-        <v>31</v>
+        <v>51</v>
       </c>
       <c r="D1" t="s">
         <v>6</v>
@@ -701,19 +845,19 @@
         <v>8</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>11</v>
+        <v>52</v>
       </c>
       <c r="G1" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="H1" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="I1" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="J1" t="s">
-        <v>27</v>
+        <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:10">
@@ -724,7 +868,7 @@
         <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="D2" t="s">
         <v>7</v>
@@ -733,19 +877,19 @@
         <v>9</v>
       </c>
       <c r="F2" t="s">
-        <v>12</v>
+        <v>53</v>
       </c>
       <c r="G2" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="H2" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="I2" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="J2" t="s">
-        <v>28</v>
+        <v>36</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -756,7 +900,7 @@
         <v>5</v>
       </c>
       <c r="C3" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="D3" t="s">
         <v>7</v>
@@ -765,19 +909,19 @@
         <v>9</v>
       </c>
       <c r="F3" t="s">
-        <v>13</v>
+        <v>54</v>
       </c>
       <c r="G3" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="H3" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="I3" t="s">
-        <v>26</v>
+        <v>34</v>
       </c>
       <c r="J3" t="s">
-        <v>29</v>
+        <v>37</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -788,7 +932,7 @@
         <v>4</v>
       </c>
       <c r="C4" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="D4" t="s">
         <v>7</v>
@@ -797,19 +941,19 @@
         <v>10</v>
       </c>
       <c r="F4" t="s">
-        <v>14</v>
+        <v>55</v>
       </c>
       <c r="G4" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="H4" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="I4" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="J4" t="s">
-        <v>28</v>
+        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>